<commit_message>
Incluida busca no Tauste
</commit_message>
<xml_diff>
--- a/confiança.xlsx
+++ b/confiança.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R$ 1,49</t>
+          <t>R$ 1,69</t>
         </is>
       </c>
     </row>
@@ -496,48 +496,48 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Água Mineral Frescca com Gás 510ml</t>
+          <t>Refrigerante Guaraná Antarctica Zero Garrafa 200ML</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R$ 1,75</t>
+          <t>R$ 1,65</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cerveja Heineken Premium Long Neck 330ml</t>
+          <t>Água Mineral sem Gás Frescca 1,5 Litros</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R$ 5,29</t>
+          <t>R$ 2,29</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Água Mineral sem Gás Frescca 1,5 Litros</t>
+          <t>Refrigerante Guaraná Antarctica 200ML Garrafa Pet</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R$ 2,29</t>
+          <t>R$ 1,65</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Cerveja Império Puro Malte Lata 269ml</t>
+          <t>Refrigerante Coca-Cola Sem Açúcar Lata 220ml</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R$ 2,49</t>
+          <t>R$ 2,69</t>
         </is>
       </c>
     </row>
@@ -556,360 +556,348 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Cerveja Budweiser American Lager 350ml Lata</t>
+          <t>Refrigerante Coca-Cola Sem Açúcar 1,5 litros</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R$ 3,59</t>
+          <t>R$ 8,29</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Refrigerante Coca-Cola Sem Açúcar Lata 220ml</t>
+          <t>Suco de Maçã Yakult 200ml</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>R$ 2,69</t>
+          <t>R$ 2,97</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Cerveja Heineken Lata 350ml</t>
+          <t>Água Mineral com Gás Prata 510ml</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>R$ 5,79</t>
+          <t>R$ 2,39</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Refrigerante Coca-Cola Sem Açúcar 1,5 litros</t>
+          <t>Cerveja Budweiser American Lager 350ml Lata</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R$ 8,29</t>
+          <t>R$ 3,78</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Refrigerante Coca-Cola Sem Açúcar 1 Litro</t>
+          <t>Água Mineral Frescca com Gás 1,5L</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>R$ 6,39</t>
+          <t>R$ 2,39</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Água Mineral Frescca com Gás 1,5L</t>
+          <t>Bebida Maguary Fruit Shoot 100% Suco Uva TP 150ml</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>R$ 2,39</t>
+          <t>R$ 2,18</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Água Mineral com Gás Crystal 500ml</t>
+          <t>Água Mineral Cristal Select sem Gás 500ml</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>R$ 2,59</t>
+          <t>R$ 1,29</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Refrigerante Guaraná Antarctica 200ML Garrafa Pet</t>
+          <t>Refrigerante Coca-Cola Lata 220ml</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>R$ 1,65</t>
+          <t>R$ 2,69</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Cerveja Amstel Puro Malte Lata 350ml</t>
+          <t>Refrigerante Coca Cola Original 2L</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>R$ 3,99</t>
+          <t>R$ 10,29</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Suco de Uva Del Valle Kapo 200ml</t>
+          <t>Refrigerante Guaraná Antarctica Sem Açúcar 350ml Lata</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>R$ 2,38</t>
+          <t>R$ 3,19</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Refrigerante Antarctica Guaraná sem açúcar 200ml</t>
+          <t>Refrigerante Coca-Cola Sem Açúcar 1 Litro</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>R$ 1,65</t>
+          <t>R$ 6,39</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Água Mineral Prata Com Gás 370Ml</t>
+          <t>Água Mineral com Gás Crystal 500ml</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>R$ 2,89</t>
+          <t>R$ 2,59</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Suco de Maçã Yakult 200ml</t>
+          <t>Refrigerante Coca-Cola Sem Açúcar 600ml</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>R$ 3,29</t>
+          <t>R$ 4,79</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Refrigerante Guaraná Antarctica Sem Açúcar 350ml Lata</t>
+          <t>Cerveja Petra Puro Malte 350ml</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>R$ 3,09</t>
+          <t>R$ 3,29</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Refrigerante Coca-Cola Sem Açúcar 600ml</t>
+          <t>Cerveja Heineken Original Long Neck 250ml</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>R$ 4,79</t>
+          <t>R$ 5,29</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Bebida Maguary Fruit Shoot 100% Suco Uva TP 150ml</t>
+          <t>Água Mineral Natural Prata Sem Gás 370Ml</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>R$ 1,94</t>
+          <t>R$ 2,39</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Refrigerante Pepsi Black Cola Zero 2 Litros</t>
+          <t>Refrigerante Limoneto H2OH! 500ml</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>R$ 7,79</t>
+          <t>R$ 3,95</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Água Mineral com Gás Prata 510ml</t>
+          <t>Suco de Morango Del Valle Kapo 200ml</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>R$ 2,44</t>
+          <t>R$ 2,39</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Água Mineral sem Gás Prata 510ml</t>
+          <t>Cerveja Heineken Premium Long Neck 330ml</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>R$ 2,39</t>
+          <t>R$ 5,98</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Refrigerante Coca-Cola Sem Açúcar Lata 350ml</t>
+          <t>Água Mineral Prata Com Gás 370Ml</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>R$ 3,69</t>
+          <t>R$ 2,89</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Água Mineral Natural Minalba sem Gás 510ml</t>
+          <t>Cerveja Amstel Puro Malte Lata 350ml</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>R$ 1,79</t>
+          <t>R$ 3,99</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Cerveja Original Pilsen 350ml</t>
+          <t>Água Mineral Sferriê com Gás 510ml</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>R$ 4,59</t>
+          <t>R$ 1,98</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Água Mineral Natural Prata Sem Gás 370Ml</t>
+          <t>Água Mineral Natural Minalba sem Gás 510ml</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>R$ 2,39</t>
+          <t>R$ 1,75</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Refrigerante Coca Cola Original 2L</t>
+          <t>Refrigerante Coca-Cola 600ml</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>R$ 10,29</t>
+          <t>R$ 4,79</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Refrigerante Coca-Cola 600ml</t>
+          <t>Cerveja Budweiser Zero Álcool Lata 350ml</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>R$ 4,79</t>
+          <t>R$ 3,99</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Água Mineral Sferrie sem Gás 510ml</t>
+          <t>Refrigerante Pepsi Black Cola Zero 2 Litros</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>R$ 1,75</t>
+          <t>R$ 7,19</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Refrigerante Coca-Cola Lata 220ml</t>
+          <t>Suco Maguary Fruit Shoot 100% Maçã 150ml</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>R$ 2,69</t>
+          <t>R$ 2,18</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Cerveja Heineken Original Lata 269ml</t>
+          <t>Cerveja Heineken Original Lata 473ml</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>R$ 4,49</t>
+          <t>R$ 6,48</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Suco de Morango Del Valle Kapo 200ml</t>
+          <t>Cerveja Heineken Lata 350ml</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>R$ 2,38</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Cerveja Spaten Puro Malte Lata 350ml</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>R$ 4,19</t>
+          <t>R$ 5,69</t>
         </is>
       </c>
     </row>

</xml_diff>